<commit_message>
added multiple data provider and mastert suite testng file for execution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CustomerSuite.xlsx
+++ b/src/test/resources/testdata/CustomerSuite.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A7D6ED6-FAA4-41AE-A762-A2AD657ADA4D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2D507B-4298-4407-A229-7FBEA8E942EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{C43DA6B6-F12F-460F-93F6-92CAD3B66125}"/>
+    <workbookView xWindow="36780" yWindow="3000" windowWidth="20820" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,6 +29,71 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>manish</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>P6767</t>
+  </si>
+  <si>
+    <t>X7878</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>manish k</t>
+  </si>
+  <si>
+    <t>jyoti</t>
+  </si>
+  <si>
+    <t>jyoti k</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,13 +442,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAD363B-3E21-4C88-93D1-A8B5ACDAF37B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A26B2B-C290-4CD6-AC1F-130AC29407C7}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>